<commit_message>
prestatus 1: one excel workbook, initializer added, module 2_3 to be done
</commit_message>
<xml_diff>
--- a/exe/FinancialRecords_Template.xlsx
+++ b/exe/FinancialRecords_Template.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\9_Vinager\exe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DFEE73-FC78-49DB-8CBD-8924A5DE6A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8D6F2E3-FAD7-4107-BE32-4B0CF15AF8C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet" sheetId="2" r:id="rId1"/>
     <sheet name="Income" sheetId="3" r:id="rId2"/>
     <sheet name="Expenses" sheetId="4" r:id="rId3"/>
     <sheet name="Records" sheetId="5" r:id="rId4"/>
+    <sheet name="Accounts &amp; Wealth" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -575,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N23" sqref="N23:N27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -653,7 +654,10 @@
       <c r="N2" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="4"/>
+      <c r="P2" s="4">
+        <f>N7</f>
+        <v>0</v>
+      </c>
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
     </row>
@@ -673,7 +677,10 @@
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
+      <c r="N3" s="4">
+        <f>SUM(B3:M3)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -691,7 +698,10 @@
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+      <c r="N4" s="4">
+        <f>SUM(B4:M4)</f>
+        <v>0</v>
+      </c>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
@@ -755,7 +765,10 @@
       <c r="K7" s="8"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
+      <c r="N7" s="4">
+        <f>SUM(B7:M7)</f>
+        <v>0</v>
+      </c>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="14"/>
@@ -1681,7 +1694,10 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="N2" s="4">
+        <f>SUM(B2:M2)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -2140,7 +2156,10 @@
       <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
+      <c r="N2" s="4">
+        <f>SUM(B2:M2)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -2564,4 +2583,18 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FAFF5AA-620F-4631-A5E3-7115759263A0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Wealth Allocation: border styling
</commit_message>
<xml_diff>
--- a/exe/FinancialRecords_Template.xlsx
+++ b/exe/FinancialRecords_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\9_Vinager\exe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8832ACA-958C-4024-97CC-DE01DA7141CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B9884E6-CA5D-4723-999A-C738F4FEA2A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{18A8FA7E-DCA9-4CD3-B68E-6009C6A4BCE4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{18A8FA7E-DCA9-4CD3-B68E-6009C6A4BCE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Financial Statement" sheetId="1" r:id="rId1"/>
@@ -645,13 +645,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F324A22D-CBB2-497A-AD6B-363E6C8102A4}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
@@ -819,68 +822,84 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="10"/>
+    </row>
     <row r="11" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="10"/>
-    </row>
-    <row r="12" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="1" t="s">
+      <c r="A11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="L11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N12" s="3" t="s">
+      <c r="N11" s="3" t="s">
         <v>14</v>
       </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" s="4"/>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="4"/>
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
@@ -898,110 +917,94 @@
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-      <c r="L14" s="4"/>
-      <c r="M14" s="4"/>
-      <c r="N14" s="4"/>
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="6"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="6"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-    </row>
-    <row r="16" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="8" t="s">
+      <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="M16" s="9"/>
-      <c r="N16" s="10"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="10"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
-      <c r="K17" s="7"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
+      <c r="A17" s="5"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5"/>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
-      <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="5"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="4"/>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="4"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="A6:N6"/>
-    <mergeCell ref="A11:N11"/>
-    <mergeCell ref="A16:N16"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="A15:N15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1012,7 +1015,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1221,7 +1224,7 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1327,7 +1330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD2EAE5-3ADB-41A2-9EDC-2E3A64919A00}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Delete bordering by default
-adding date destroys border
-test the functionality of each commands once again
</commit_message>
<xml_diff>
--- a/exe/FinancialRecords_Template.xlsx
+++ b/exe/FinancialRecords_Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\9_Vinager\exe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05E6C0C-435A-4A37-8126-AC233D2EDEF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C902FFD-D9EC-4135-BB0D-945604979482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{18A8FA7E-DCA9-4CD3-B68E-6009C6A4BCE4}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{18A8FA7E-DCA9-4CD3-B68E-6009C6A4BCE4}"/>
   </bookViews>
   <sheets>
     <sheet name="Income Statement" sheetId="1" r:id="rId1"/>
@@ -164,7 +164,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -225,62 +225,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -306,32 +250,17 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -341,10 +270,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -664,33 +593,33 @@
   <dimension ref="A1:N22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:N10"/>
+      <selection activeCell="A15" sqref="A15:N15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
-    </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="8"/>
+    </row>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -734,25 +663,25 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="11"/>
-      <c r="M3" s="11"/>
-      <c r="N3" s="12"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -766,9 +695,9 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="4"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="N4" s="5"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
@@ -784,7 +713,7 @@
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -800,7 +729,7 @@
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -816,7 +745,7 @@
       <c r="M7" s="5"/>
       <c r="N7" s="5"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="5"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -832,7 +761,7 @@
       <c r="M8" s="5"/>
       <c r="N8" s="5"/>
     </row>
-    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -848,41 +777,41 @@
       <c r="M9" s="5"/>
       <c r="N9" s="5"/>
     </row>
-    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="11"/>
-      <c r="N10" s="12"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="7"/>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
-      <c r="K11" s="7"/>
-      <c r="L11" s="7"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="4"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="8"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -898,7 +827,7 @@
       <c r="M12" s="5"/>
       <c r="N12" s="5"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -914,7 +843,7 @@
       <c r="M13" s="5"/>
       <c r="N13" s="5"/>
     </row>
-    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -930,43 +859,43 @@
       <c r="M14" s="5"/>
       <c r="N14" s="5"/>
     </row>
-    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="12"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="8"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="4"/>
-      <c r="M16" s="4"/>
-      <c r="N16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5"/>
+      <c r="M16" s="5"/>
+      <c r="N16" s="5"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -982,27 +911,27 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
       <c r="M17" s="5"/>
-      <c r="N17" s="4"/>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A18" s="6" t="s">
+      <c r="N17" s="5"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="9"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
@@ -1018,53 +947,53 @@
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A20" s="8"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="8"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A21" s="8"/>
-      <c r="B21" s="8"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="N21" s="8"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A22" s="8"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="8"/>
-      <c r="M22" s="8"/>
-      <c r="N22" s="8"/>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="4"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="4"/>
+      <c r="B21" s="4"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="4"/>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="4"/>
+      <c r="M22" s="4"/>
+      <c r="N22" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1081,39 +1010,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B75D356C-2BAE-4DB6-9B80-B3F23FD63E2D}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="12"/>
-      <c r="G1" s="13" t="s">
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+      <c r="G1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="H1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="11"/>
-      <c r="K1" s="12"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="8"/>
       <c r="M1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1121,9 +1050,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="14"/>
-      <c r="B2" s="14"/>
+    <row r="2" spans="1:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
       <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1133,8 +1062,8 @@
       <c r="E2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
       <c r="I2" s="1" t="s">
         <v>22</v>
       </c>
@@ -1144,34 +1073,40 @@
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
-      <c r="E3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="5"/>
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
-      <c r="K3" s="4"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1191,15 +1126,15 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="6" max="6" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1219,15 +1154,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>

</xml_diff>